<commit_message>
Adicionado dia e horario no CSV
</commit_message>
<xml_diff>
--- a/Python/Gráficos.xlsx
+++ b/Python/Gráficos.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="testeCSV" localSheetId="0">Sheet1!$A$1:$E$50</definedName>
+    <definedName name="testeCSV_1" localSheetId="0">Sheet1!$A$1:$F$65</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -22,7 +22,8 @@
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="testeCSV" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\lucap\Documents\GitHub\TCC-LoRa\Python\testeCSV.csv" tab="0" comma="1">
-      <textFields count="5">
+      <textFields count="6">
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
   <si>
     <t>Temperatura</t>
   </si>
@@ -46,306 +47,208 @@
     <t>Pressao</t>
   </si>
   <si>
-    <t>Data</t>
-  </si>
-  <si>
     <t>Dados HEX</t>
   </si>
   <si>
-    <t>2016-06-09T12:38:52.634Z</t>
-  </si>
-  <si>
     <t>0085022D03A5</t>
   </si>
   <si>
-    <t>2016-06-09T12:54:47.770Z</t>
-  </si>
-  <si>
     <t>0083023603A4</t>
   </si>
   <si>
-    <t>2016-06-09T13:10:43.134Z</t>
-  </si>
-  <si>
     <t>0083022903A4</t>
   </si>
   <si>
-    <t>2016-06-09T13:26:38.516Z</t>
-  </si>
-  <si>
     <t>0085023503A4</t>
   </si>
   <si>
-    <t>2016-06-09T13:42:34.019Z</t>
-  </si>
-  <si>
     <t>0086023503A4</t>
   </si>
   <si>
-    <t>2016-06-09T13:58:29.309Z</t>
-  </si>
-  <si>
     <t>0087022703A4</t>
   </si>
   <si>
-    <t>2016-06-09T14:14:25.358Z</t>
-  </si>
-  <si>
     <t>0088022403A4</t>
   </si>
   <si>
-    <t>2016-06-09T14:30:20.063Z</t>
-  </si>
-  <si>
     <t>008B021B03A3</t>
   </si>
   <si>
-    <t>2016-06-09T14:46:15.476Z</t>
-  </si>
-  <si>
     <t>008A021303A3</t>
   </si>
   <si>
-    <t>2016-06-09T15:02:10.867Z</t>
-  </si>
-  <si>
     <t>008F020503A3</t>
   </si>
   <si>
-    <t>2016-06-09T15:18:06.258Z</t>
-  </si>
-  <si>
     <t>0091020703A3</t>
   </si>
   <si>
-    <t>2016-06-09T15:34:01.650Z</t>
-  </si>
-  <si>
     <t>0093020003A2</t>
   </si>
   <si>
-    <t>2016-06-09T15:49:57.061Z</t>
-  </si>
-  <si>
     <t>009501F603A2</t>
   </si>
   <si>
-    <t>2016-06-09T16:05:52.458Z</t>
-  </si>
-  <si>
     <t>009701F503A2</t>
   </si>
   <si>
-    <t>2016-06-09T16:21:47.864Z</t>
-  </si>
-  <si>
     <t>009901F403A2</t>
   </si>
   <si>
-    <t>2016-06-09T16:37:43.853Z</t>
-  </si>
-  <si>
     <t>009C01EA03A2</t>
   </si>
   <si>
-    <t>2016-06-09T16:53:38.714Z</t>
-  </si>
-  <si>
     <t>009F01DF03A2</t>
   </si>
   <si>
-    <t>2016-06-09T17:09:34.078Z</t>
-  </si>
-  <si>
     <t>009E01EE03A0</t>
   </si>
   <si>
-    <t>2016-06-09T17:25:29.475Z</t>
-  </si>
-  <si>
     <t>009F01EF03A0</t>
   </si>
   <si>
-    <t>2016-06-09T17:41:24.891Z</t>
-  </si>
-  <si>
     <t>009F01EB03A0</t>
   </si>
   <si>
-    <t>2016-06-09T17:57:20.293Z</t>
-  </si>
-  <si>
     <t>00A001F103A2</t>
   </si>
   <si>
-    <t>2016-06-09T18:13:15.699Z</t>
-  </si>
-  <si>
     <t>00A101E603A2</t>
   </si>
   <si>
-    <t>2016-06-09T18:29:11.105Z</t>
-  </si>
-  <si>
     <t>00A201E903A0</t>
   </si>
   <si>
-    <t>2016-06-09T18:45:06.518Z</t>
-  </si>
-  <si>
     <t>00A201EB03A2</t>
   </si>
   <si>
-    <t>2016-06-09T19:01:01.918Z</t>
-  </si>
-  <si>
     <t>00A201ED03A0</t>
   </si>
   <si>
-    <t>2016-06-09T19:16:57.316Z</t>
-  </si>
-  <si>
     <t>00A001EE03A2</t>
   </si>
   <si>
-    <t>2016-06-09T19:32:52.727Z</t>
-  </si>
-  <si>
     <t>00A001EC03A2</t>
   </si>
   <si>
-    <t>2016-06-09T19:48:48.130Z</t>
-  </si>
-  <si>
     <t>00A101E703A2</t>
   </si>
   <si>
-    <t>2016-06-09T20:04:43.535Z</t>
-  </si>
-  <si>
     <t>009F01E303A2</t>
   </si>
   <si>
-    <t>2016-06-09T20:20:38.926Z</t>
-  </si>
-  <si>
-    <t>2016-06-09T20:36:34.330Z</t>
-  </si>
-  <si>
     <t>009B01F403A2</t>
   </si>
   <si>
-    <t>2016-06-09T20:52:29.722Z</t>
-  </si>
-  <si>
     <t>009801F603A2</t>
   </si>
   <si>
-    <t>2016-06-09T21:08:25.152Z</t>
-  </si>
-  <si>
     <t>009901F703A2</t>
   </si>
   <si>
-    <t>2016-06-09T21:24:20.543Z</t>
-  </si>
-  <si>
     <t>009901F103A2</t>
   </si>
   <si>
-    <t>2016-06-09T21:40:15.939Z</t>
-  </si>
-  <si>
     <t>009601ED03A2</t>
   </si>
   <si>
-    <t>2016-06-09T21:56:11.339Z</t>
-  </si>
-  <si>
     <t>009501F403A3</t>
   </si>
   <si>
-    <t>2016-06-09T22:12:06.729Z</t>
-  </si>
-  <si>
     <t>009201F703A2</t>
   </si>
   <si>
-    <t>2016-06-09T22:28:02.131Z</t>
-  </si>
-  <si>
     <t>009101FB03A3</t>
   </si>
   <si>
-    <t>2016-06-09T22:43:57.527Z</t>
-  </si>
-  <si>
-    <t>2016-06-09T22:59:52.933Z</t>
-  </si>
-  <si>
     <t>009001FD03A3</t>
   </si>
   <si>
-    <t>2016-06-09T23:15:48.316Z</t>
-  </si>
-  <si>
     <t>008E020403A3</t>
   </si>
   <si>
-    <t>2016-06-09T23:31:43.719Z</t>
-  </si>
-  <si>
     <t>008D020B03A3</t>
   </si>
   <si>
-    <t>2016-06-09T23:47:39.443Z</t>
-  </si>
-  <si>
     <t>008D020403A3</t>
   </si>
   <si>
-    <t>2016-06-10T00:03:34.500Z</t>
-  </si>
-  <si>
     <t>008B020A03A3</t>
   </si>
   <si>
-    <t>2016-06-10T00:19:29.887Z</t>
-  </si>
-  <si>
     <t>008A020A03A3</t>
   </si>
   <si>
-    <t>2016-06-10T00:35:25.279Z</t>
-  </si>
-  <si>
     <t>008A020E03A3</t>
   </si>
   <si>
-    <t>2016-06-10T00:51:20.666Z</t>
-  </si>
-  <si>
     <t>0089020D03A3</t>
   </si>
   <si>
-    <t>2016-06-10T01:07:16.067Z</t>
-  </si>
-  <si>
     <t>0087020D03A3</t>
   </si>
   <si>
-    <t>2016-06-10T01:23:11.445Z</t>
-  </si>
-  <si>
     <t>0086020D03A3</t>
+  </si>
+  <si>
+    <t>0085021003A2</t>
+  </si>
+  <si>
+    <t>0084021303A3</t>
+  </si>
+  <si>
+    <t>0083021503A3</t>
+  </si>
+  <si>
+    <t>0083021903A3</t>
+  </si>
+  <si>
+    <t>0082021903A3</t>
+  </si>
+  <si>
+    <t>0081021A03A3</t>
+  </si>
+  <si>
+    <t>0080021C03A3</t>
+  </si>
+  <si>
+    <t>0080021F03A3</t>
+  </si>
+  <si>
+    <t>007F022303A3</t>
+  </si>
+  <si>
+    <t>007E022503A2</t>
+  </si>
+  <si>
+    <t>007D022A03A2</t>
+  </si>
+  <si>
+    <t>007C022B03A2</t>
+  </si>
+  <si>
+    <t>007B022C03A2</t>
+  </si>
+  <si>
+    <t>0079023103A2</t>
+  </si>
+  <si>
+    <t>0077023703A2</t>
+  </si>
+  <si>
+    <t>Dia</t>
+  </si>
+  <si>
+    <t>Hora</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -384,12 +287,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -444,169 +349,212 @@
             </c:strRef>
           </c:tx>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$D:$D</c:f>
-              <c:strCache>
-                <c:ptCount val="50"/>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$1048576</c:f>
+              <c:numCache>
+                <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
+                <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>Data</c:v>
+                  <c:v>0.52700231481481474</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2016-06-09T12:38:52.634Z</c:v>
+                  <c:v>0.53805289351851848</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2016-06-09T12:54:47.770Z</c:v>
+                  <c:v>0.54911034722222218</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2016-06-09T13:10:43.134Z</c:v>
+                  <c:v>0.56016800925925925</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2016-06-09T13:26:38.516Z</c:v>
+                  <c:v>0.57122707175925924</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2016-06-09T13:42:34.019Z</c:v>
+                  <c:v>0.58228366898148154</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2016-06-09T13:58:29.309Z</c:v>
+                  <c:v>0.59334905092592594</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2016-06-09T14:14:25.358Z</c:v>
+                  <c:v>0.60439887731481479</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2016-06-09T14:30:20.063Z</c:v>
+                  <c:v>0.61545689814814819</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2016-06-09T14:46:15.476Z</c:v>
+                  <c:v>0.62651466435185188</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2016-06-09T15:02:10.867Z</c:v>
+                  <c:v>0.63757243055555557</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2016-06-09T15:18:06.258Z</c:v>
+                  <c:v>0.6486302083333334</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2016-06-09T15:34:01.650Z</c:v>
+                  <c:v>0.65968820601851852</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2016-06-09T15:49:57.061Z</c:v>
+                  <c:v>0.67074604166666674</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2016-06-09T16:05:52.458Z</c:v>
+                  <c:v>0.68180398148148147</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2016-06-09T16:21:47.864Z</c:v>
+                  <c:v>0.69286866898148147</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2016-06-09T16:37:43.853Z</c:v>
+                  <c:v>0.70392030092592595</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2016-06-09T16:53:38.714Z</c:v>
+                  <c:v>0.71497775462962965</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2016-06-09T17:09:34.078Z</c:v>
+                  <c:v>0.72603559027777775</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2016-06-09T17:25:29.475Z</c:v>
+                  <c:v>0.73709364583333337</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2016-06-09T17:41:24.891Z</c:v>
+                  <c:v>0.74815153935185175</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2016-06-09T17:57:20.293Z</c:v>
+                  <c:v>0.7592094791666667</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2016-06-09T18:13:15.699Z</c:v>
+                  <c:v>0.77026741898148154</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2016-06-09T18:29:11.105Z</c:v>
+                  <c:v>0.78132543981481473</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2016-06-09T18:45:06.518Z</c:v>
+                  <c:v>0.79238331018518515</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2016-06-09T19:01:01.918Z</c:v>
+                  <c:v>0.8034411574074074</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2016-06-09T19:16:57.316Z</c:v>
+                  <c:v>0.81449915509259263</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2016-06-09T19:32:52.727Z</c:v>
+                  <c:v>0.82555706018518515</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2016-06-09T19:48:48.130Z</c:v>
+                  <c:v>0.83661498842592597</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2016-06-09T20:04:43.535Z</c:v>
+                  <c:v>0.84767275462962965</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2016-06-09T20:20:38.926Z</c:v>
+                  <c:v>0.85873067129629632</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2016-06-09T20:36:34.330Z</c:v>
+                  <c:v>0.86978844907407404</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2016-06-09T20:52:29.722Z</c:v>
+                  <c:v>0.88084666666666667</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2016-06-09T21:08:25.152Z</c:v>
+                  <c:v>0.89190443287037036</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2016-06-09T21:24:20.543Z</c:v>
+                  <c:v>0.90296225694444443</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2016-06-09T21:40:15.939Z</c:v>
+                  <c:v>0.91402012731481486</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2016-06-09T21:56:11.339Z</c:v>
+                  <c:v>0.92507788194444451</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2016-06-09T22:12:06.729Z</c:v>
+                  <c:v>0.93613577546296289</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2016-06-09T22:28:02.131Z</c:v>
+                  <c:v>0.94719359953703697</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2016-06-09T22:43:57.527Z</c:v>
+                  <c:v>0.95825153935185181</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2016-06-09T22:59:52.933Z</c:v>
+                  <c:v>0.96930921296296291</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2016-06-09T23:15:48.316Z</c:v>
+                  <c:v>0.98036711805555565</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2016-06-09T23:31:43.719Z</c:v>
+                  <c:v>0.99142873842592583</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2016-06-09T23:47:39.443Z</c:v>
+                  <c:v>2.4826388888888888E-3</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2016-06-10T00:03:34.500Z</c:v>
+                  <c:v>1.3540358796296297E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2016-06-10T00:19:29.887Z</c:v>
+                  <c:v>2.4598136574074076E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2016-06-10T00:35:25.279Z</c:v>
+                  <c:v>3.5655856481481486E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2016-06-10T00:51:20.666Z</c:v>
+                  <c:v>4.6713738425925931E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2016-06-10T01:07:16.067Z</c:v>
+                  <c:v>5.7771354166666671E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2016-06-10T01:23:11.445Z</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>6.882907407407407E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>7.9886817129629625E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>9.0944594907407403E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.10200362268518519</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.11305983796296297</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.12412620370370371</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.13517533564814815</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.14623340277777777</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.15729067129629629</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.16834828703703705</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.17940592592592594</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.19046371527777781</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.20152120370370372</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.21257873842592592</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.2236363888888889</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$50</c:f>
+              <c:f>Sheet1!$B$2:$B$65</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:ptCount val="64"/>
                 <c:pt idx="0">
                   <c:v>55.7</c:v>
                 </c:pt>
@@ -753,6 +701,51 @@
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>52.5</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>52.8</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>53.1</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>53.3</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53.7</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>53.7</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>53.8</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>54.3</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>54.7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>54.9</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>55.4</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>55.5</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>55.6</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>56.1</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>56.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -779,7 +772,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="@" sourceLinked="1"/>
+        <c:numFmt formatCode="[$-F400]h:mm:ss\ AM/PM" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -858,170 +851,213 @@
             </c:strRef>
           </c:tx>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$D:$D</c:f>
-              <c:strCache>
-                <c:ptCount val="50"/>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$1048576</c:f>
+              <c:numCache>
+                <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
+                <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>Data</c:v>
+                  <c:v>0.52700231481481474</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2016-06-09T12:38:52.634Z</c:v>
+                  <c:v>0.53805289351851848</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2016-06-09T12:54:47.770Z</c:v>
+                  <c:v>0.54911034722222218</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2016-06-09T13:10:43.134Z</c:v>
+                  <c:v>0.56016800925925925</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2016-06-09T13:26:38.516Z</c:v>
+                  <c:v>0.57122707175925924</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2016-06-09T13:42:34.019Z</c:v>
+                  <c:v>0.58228366898148154</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2016-06-09T13:58:29.309Z</c:v>
+                  <c:v>0.59334905092592594</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2016-06-09T14:14:25.358Z</c:v>
+                  <c:v>0.60439887731481479</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2016-06-09T14:30:20.063Z</c:v>
+                  <c:v>0.61545689814814819</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2016-06-09T14:46:15.476Z</c:v>
+                  <c:v>0.62651466435185188</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2016-06-09T15:02:10.867Z</c:v>
+                  <c:v>0.63757243055555557</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2016-06-09T15:18:06.258Z</c:v>
+                  <c:v>0.6486302083333334</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2016-06-09T15:34:01.650Z</c:v>
+                  <c:v>0.65968820601851852</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2016-06-09T15:49:57.061Z</c:v>
+                  <c:v>0.67074604166666674</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2016-06-09T16:05:52.458Z</c:v>
+                  <c:v>0.68180398148148147</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2016-06-09T16:21:47.864Z</c:v>
+                  <c:v>0.69286866898148147</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2016-06-09T16:37:43.853Z</c:v>
+                  <c:v>0.70392030092592595</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2016-06-09T16:53:38.714Z</c:v>
+                  <c:v>0.71497775462962965</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2016-06-09T17:09:34.078Z</c:v>
+                  <c:v>0.72603559027777775</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2016-06-09T17:25:29.475Z</c:v>
+                  <c:v>0.73709364583333337</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2016-06-09T17:41:24.891Z</c:v>
+                  <c:v>0.74815153935185175</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2016-06-09T17:57:20.293Z</c:v>
+                  <c:v>0.7592094791666667</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2016-06-09T18:13:15.699Z</c:v>
+                  <c:v>0.77026741898148154</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2016-06-09T18:29:11.105Z</c:v>
+                  <c:v>0.78132543981481473</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2016-06-09T18:45:06.518Z</c:v>
+                  <c:v>0.79238331018518515</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2016-06-09T19:01:01.918Z</c:v>
+                  <c:v>0.8034411574074074</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2016-06-09T19:16:57.316Z</c:v>
+                  <c:v>0.81449915509259263</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2016-06-09T19:32:52.727Z</c:v>
+                  <c:v>0.82555706018518515</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2016-06-09T19:48:48.130Z</c:v>
+                  <c:v>0.83661498842592597</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2016-06-09T20:04:43.535Z</c:v>
+                  <c:v>0.84767275462962965</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2016-06-09T20:20:38.926Z</c:v>
+                  <c:v>0.85873067129629632</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2016-06-09T20:36:34.330Z</c:v>
+                  <c:v>0.86978844907407404</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2016-06-09T20:52:29.722Z</c:v>
+                  <c:v>0.88084666666666667</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2016-06-09T21:08:25.152Z</c:v>
+                  <c:v>0.89190443287037036</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2016-06-09T21:24:20.543Z</c:v>
+                  <c:v>0.90296225694444443</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2016-06-09T21:40:15.939Z</c:v>
+                  <c:v>0.91402012731481486</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2016-06-09T21:56:11.339Z</c:v>
+                  <c:v>0.92507788194444451</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2016-06-09T22:12:06.729Z</c:v>
+                  <c:v>0.93613577546296289</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2016-06-09T22:28:02.131Z</c:v>
+                  <c:v>0.94719359953703697</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2016-06-09T22:43:57.527Z</c:v>
+                  <c:v>0.95825153935185181</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2016-06-09T22:59:52.933Z</c:v>
+                  <c:v>0.96930921296296291</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2016-06-09T23:15:48.316Z</c:v>
+                  <c:v>0.98036711805555565</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2016-06-09T23:31:43.719Z</c:v>
+                  <c:v>0.99142873842592583</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2016-06-09T23:47:39.443Z</c:v>
+                  <c:v>2.4826388888888888E-3</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2016-06-10T00:03:34.500Z</c:v>
+                  <c:v>1.3540358796296297E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2016-06-10T00:19:29.887Z</c:v>
+                  <c:v>2.4598136574074076E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2016-06-10T00:35:25.279Z</c:v>
+                  <c:v>3.5655856481481486E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2016-06-10T00:51:20.666Z</c:v>
+                  <c:v>4.6713738425925931E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2016-06-10T01:07:16.067Z</c:v>
+                  <c:v>5.7771354166666671E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2016-06-10T01:23:11.445Z</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>6.882907407407407E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>7.9886817129629625E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>9.0944594907407403E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.10200362268518519</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.11305983796296297</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.12412620370370371</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.13517533564814815</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.14623340277777777</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.15729067129629629</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.16834828703703705</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.17940592592592594</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.19046371527777781</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.20152120370370372</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.21257873842592592</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.2236363888888889</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$50</c:f>
+              <c:f>Sheet1!$A$2:$A$65</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="49"/>
-                <c:pt idx="0" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)">
+                <c:ptCount val="64"/>
+                <c:pt idx="0">
                   <c:v>13.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -1167,6 +1203,51 @@
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>13.4</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>13.3</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>13.2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>13.1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>13.1</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>12.9</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>12.8</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>12.8</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>12.7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>12.6</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>12.4</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>12.3</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>11.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1183,21 +1264,21 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="197925120"/>
-        <c:axId val="197926912"/>
+        <c:axId val="198252800"/>
+        <c:axId val="198254592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="197925120"/>
+        <c:axId val="198252800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="@" sourceLinked="1"/>
+        <c:numFmt formatCode="[$-F400]h:mm:ss\ AM/PM" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="197926912"/>
+        <c:crossAx val="198254592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1205,18 +1286,18 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="197926912"/>
+        <c:axId val="198254592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="197925120"/>
+        <c:crossAx val="198252800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1272,169 +1353,212 @@
             </c:strRef>
           </c:tx>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$D:$D</c:f>
-              <c:strCache>
-                <c:ptCount val="50"/>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$1048576</c:f>
+              <c:numCache>
+                <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
+                <c:ptCount val="1048575"/>
                 <c:pt idx="0">
-                  <c:v>Data</c:v>
+                  <c:v>0.52700231481481474</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2016-06-09T12:38:52.634Z</c:v>
+                  <c:v>0.53805289351851848</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2016-06-09T12:54:47.770Z</c:v>
+                  <c:v>0.54911034722222218</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2016-06-09T13:10:43.134Z</c:v>
+                  <c:v>0.56016800925925925</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2016-06-09T13:26:38.516Z</c:v>
+                  <c:v>0.57122707175925924</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2016-06-09T13:42:34.019Z</c:v>
+                  <c:v>0.58228366898148154</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2016-06-09T13:58:29.309Z</c:v>
+                  <c:v>0.59334905092592594</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2016-06-09T14:14:25.358Z</c:v>
+                  <c:v>0.60439887731481479</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2016-06-09T14:30:20.063Z</c:v>
+                  <c:v>0.61545689814814819</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2016-06-09T14:46:15.476Z</c:v>
+                  <c:v>0.62651466435185188</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2016-06-09T15:02:10.867Z</c:v>
+                  <c:v>0.63757243055555557</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2016-06-09T15:18:06.258Z</c:v>
+                  <c:v>0.6486302083333334</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2016-06-09T15:34:01.650Z</c:v>
+                  <c:v>0.65968820601851852</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2016-06-09T15:49:57.061Z</c:v>
+                  <c:v>0.67074604166666674</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2016-06-09T16:05:52.458Z</c:v>
+                  <c:v>0.68180398148148147</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2016-06-09T16:21:47.864Z</c:v>
+                  <c:v>0.69286866898148147</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2016-06-09T16:37:43.853Z</c:v>
+                  <c:v>0.70392030092592595</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2016-06-09T16:53:38.714Z</c:v>
+                  <c:v>0.71497775462962965</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2016-06-09T17:09:34.078Z</c:v>
+                  <c:v>0.72603559027777775</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2016-06-09T17:25:29.475Z</c:v>
+                  <c:v>0.73709364583333337</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2016-06-09T17:41:24.891Z</c:v>
+                  <c:v>0.74815153935185175</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2016-06-09T17:57:20.293Z</c:v>
+                  <c:v>0.7592094791666667</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2016-06-09T18:13:15.699Z</c:v>
+                  <c:v>0.77026741898148154</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2016-06-09T18:29:11.105Z</c:v>
+                  <c:v>0.78132543981481473</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2016-06-09T18:45:06.518Z</c:v>
+                  <c:v>0.79238331018518515</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2016-06-09T19:01:01.918Z</c:v>
+                  <c:v>0.8034411574074074</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2016-06-09T19:16:57.316Z</c:v>
+                  <c:v>0.81449915509259263</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2016-06-09T19:32:52.727Z</c:v>
+                  <c:v>0.82555706018518515</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2016-06-09T19:48:48.130Z</c:v>
+                  <c:v>0.83661498842592597</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2016-06-09T20:04:43.535Z</c:v>
+                  <c:v>0.84767275462962965</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2016-06-09T20:20:38.926Z</c:v>
+                  <c:v>0.85873067129629632</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2016-06-09T20:36:34.330Z</c:v>
+                  <c:v>0.86978844907407404</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2016-06-09T20:52:29.722Z</c:v>
+                  <c:v>0.88084666666666667</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2016-06-09T21:08:25.152Z</c:v>
+                  <c:v>0.89190443287037036</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2016-06-09T21:24:20.543Z</c:v>
+                  <c:v>0.90296225694444443</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2016-06-09T21:40:15.939Z</c:v>
+                  <c:v>0.91402012731481486</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2016-06-09T21:56:11.339Z</c:v>
+                  <c:v>0.92507788194444451</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2016-06-09T22:12:06.729Z</c:v>
+                  <c:v>0.93613577546296289</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2016-06-09T22:28:02.131Z</c:v>
+                  <c:v>0.94719359953703697</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2016-06-09T22:43:57.527Z</c:v>
+                  <c:v>0.95825153935185181</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2016-06-09T22:59:52.933Z</c:v>
+                  <c:v>0.96930921296296291</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2016-06-09T23:15:48.316Z</c:v>
+                  <c:v>0.98036711805555565</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2016-06-09T23:31:43.719Z</c:v>
+                  <c:v>0.99142873842592583</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2016-06-09T23:47:39.443Z</c:v>
+                  <c:v>2.4826388888888888E-3</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2016-06-10T00:03:34.500Z</c:v>
+                  <c:v>1.3540358796296297E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2016-06-10T00:19:29.887Z</c:v>
+                  <c:v>2.4598136574074076E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2016-06-10T00:35:25.279Z</c:v>
+                  <c:v>3.5655856481481486E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2016-06-10T00:51:20.666Z</c:v>
+                  <c:v>4.6713738425925931E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2016-06-10T01:07:16.067Z</c:v>
+                  <c:v>5.7771354166666671E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2016-06-10T01:23:11.445Z</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>6.882907407407407E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>7.9886817129629625E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>9.0944594907407403E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.10200362268518519</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.11305983796296297</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.12412620370370371</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.13517533564814815</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.14623340277777777</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.15729067129629629</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.16834828703703705</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.17940592592592594</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.19046371527777781</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.20152120370370372</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.21257873842592592</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.2236363888888889</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$50</c:f>
+              <c:f>Sheet1!$C$2:$C$65</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:ptCount val="64"/>
                 <c:pt idx="0">
                   <c:v>933</c:v>
                 </c:pt>
@@ -1581,6 +1705,51 @@
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>931</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>930</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>931</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>931</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>931</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>931</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>931</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>931</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>931</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>931</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>930</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>930</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>930</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>930</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>930</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>930</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1597,21 +1766,21 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="197934464"/>
-        <c:axId val="197952640"/>
+        <c:axId val="198262144"/>
+        <c:axId val="198284416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="197934464"/>
+        <c:axId val="198262144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="@" sourceLinked="1"/>
+        <c:numFmt formatCode="[$-F400]h:mm:ss\ AM/PM" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="197952640"/>
+        <c:crossAx val="198284416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1619,7 +1788,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="197952640"/>
+        <c:axId val="198284416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1630,7 +1799,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="197934464"/>
+        <c:crossAx val="198262144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1651,16 +1820,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>57149</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1681,16 +1850,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>590549</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1711,16 +1880,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>590549</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1743,7 +1912,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="testeCSV" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="testeCSV_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2033,21 +2202,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z50"/>
+  <dimension ref="A1:Z65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB1" sqref="AB1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="26" width="9.140625" style="2"/>
+    <col min="4" max="4" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="26" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2058,14 +2230,17 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
         <v>13.3</v>
       </c>
       <c r="B2" s="3">
@@ -2074,14 +2249,17 @@
       <c r="C2" s="3">
         <v>933</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0.52700231481481474</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>13.1</v>
       </c>
@@ -2091,14 +2269,17 @@
       <c r="C3" s="3">
         <v>932</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.53805289351851848</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>13.1</v>
       </c>
@@ -2108,14 +2289,17 @@
       <c r="C4" s="3">
         <v>932</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.54911034722222218</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>13.3</v>
       </c>
@@ -2125,14 +2309,17 @@
       <c r="C5" s="3">
         <v>932</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.56016800925925925</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>13.4</v>
       </c>
@@ -2142,14 +2329,17 @@
       <c r="C6" s="3">
         <v>932</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.57122707175925924</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>13.5</v>
       </c>
@@ -2159,14 +2349,17 @@
       <c r="C7" s="3">
         <v>932</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D7" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.58228366898148154</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>13.6</v>
       </c>
@@ -2176,14 +2369,17 @@
       <c r="C8" s="3">
         <v>932</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D8" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.59334905092592594</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>13.9</v>
       </c>
@@ -2193,14 +2389,17 @@
       <c r="C9" s="3">
         <v>931</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.60439887731481479</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>13.8</v>
       </c>
@@ -2210,14 +2409,17 @@
       <c r="C10" s="3">
         <v>931</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0.61545689814814819</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>14.3</v>
       </c>
@@ -2227,14 +2429,17 @@
       <c r="C11" s="3">
         <v>931</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0.62651466435185188</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>14.5</v>
       </c>
@@ -2244,14 +2449,17 @@
       <c r="C12" s="3">
         <v>931</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0.63757243055555557</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>14.7</v>
       </c>
@@ -2261,14 +2469,17 @@
       <c r="C13" s="3">
         <v>930</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.6486302083333334</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>14.9</v>
       </c>
@@ -2278,14 +2489,17 @@
       <c r="C14" s="3">
         <v>930</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0.65968820601851852</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>15.1</v>
       </c>
@@ -2295,14 +2509,17 @@
       <c r="C15" s="3">
         <v>930</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0.67074604166666674</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15.3</v>
       </c>
@@ -2312,14 +2529,17 @@
       <c r="C16" s="3">
         <v>930</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0.68180398148148147</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>15.6</v>
       </c>
@@ -2329,14 +2549,17 @@
       <c r="C17" s="3">
         <v>930</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0.69286866898148147</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>15.9</v>
       </c>
@@ -2346,14 +2569,17 @@
       <c r="C18" s="3">
         <v>930</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0.70392030092592595</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>15.8</v>
       </c>
@@ -2363,14 +2589,17 @@
       <c r="C19" s="3">
         <v>928</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0.71497775462962965</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>15.9</v>
       </c>
@@ -2380,14 +2609,17 @@
       <c r="C20" s="3">
         <v>928</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D20" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0.72603559027777775</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>15.9</v>
       </c>
@@ -2397,14 +2629,17 @@
       <c r="C21" s="3">
         <v>928</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D21" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0.73709364583333337</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>16</v>
       </c>
@@ -2414,14 +2649,17 @@
       <c r="C22" s="3">
         <v>930</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0.74815153935185175</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>16.100000000000001</v>
       </c>
@@ -2431,14 +2669,17 @@
       <c r="C23" s="3">
         <v>930</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D23" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0.7592094791666667</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>16.2</v>
       </c>
@@ -2448,14 +2689,17 @@
       <c r="C24" s="3">
         <v>928</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D24" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0.77026741898148154</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>16.2</v>
       </c>
@@ -2465,14 +2709,17 @@
       <c r="C25" s="3">
         <v>930</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D25" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0.78132543981481473</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>16.2</v>
       </c>
@@ -2482,14 +2729,17 @@
       <c r="C26" s="3">
         <v>928</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D26" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0.79238331018518515</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>16</v>
       </c>
@@ -2499,14 +2749,17 @@
       <c r="C27" s="3">
         <v>930</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D27" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0.8034411574074074</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>16</v>
       </c>
@@ -2516,14 +2769,17 @@
       <c r="C28" s="3">
         <v>930</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D28" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E28" s="5">
+        <v>0.81449915509259263</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>16.100000000000001</v>
       </c>
@@ -2533,14 +2789,17 @@
       <c r="C29" s="3">
         <v>930</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D29" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0.82555706018518515</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>15.9</v>
       </c>
@@ -2550,14 +2809,17 @@
       <c r="C30" s="3">
         <v>930</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0.83661498842592597</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>15.6</v>
       </c>
@@ -2567,14 +2829,17 @@
       <c r="C31" s="3">
         <v>930</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D31" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E31" s="5">
+        <v>0.84767275462962965</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>15.5</v>
       </c>
@@ -2584,14 +2849,17 @@
       <c r="C32" s="3">
         <v>930</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D32" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E32" s="5">
+        <v>0.85873067129629632</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>15.2</v>
       </c>
@@ -2601,14 +2869,17 @@
       <c r="C33" s="3">
         <v>930</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D33" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E33" s="5">
+        <v>0.86978844907407404</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>15.3</v>
       </c>
@@ -2618,14 +2889,17 @@
       <c r="C34" s="3">
         <v>930</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E34" s="5">
+        <v>0.88084666666666667</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>15.3</v>
       </c>
@@ -2635,14 +2909,17 @@
       <c r="C35" s="3">
         <v>930</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E35" s="5">
+        <v>0.89190443287037036</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>15</v>
       </c>
@@ -2652,14 +2929,17 @@
       <c r="C36" s="3">
         <v>930</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E36" s="5">
+        <v>0.90296225694444443</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>14.9</v>
       </c>
@@ -2669,14 +2949,17 @@
       <c r="C37" s="3">
         <v>931</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D37" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E37" s="5">
+        <v>0.91402012731481486</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>14.6</v>
       </c>
@@ -2686,14 +2969,17 @@
       <c r="C38" s="3">
         <v>930</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D38" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E38" s="5">
+        <v>0.92507788194444451</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>14.5</v>
       </c>
@@ -2703,14 +2989,17 @@
       <c r="C39" s="3">
         <v>931</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D39" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E39" s="5">
+        <v>0.93613577546296289</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>14.5</v>
       </c>
@@ -2720,14 +3009,17 @@
       <c r="C40" s="3">
         <v>931</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D40" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E40" s="5">
+        <v>0.94719359953703697</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>14.4</v>
       </c>
@@ -2737,14 +3029,17 @@
       <c r="C41" s="3">
         <v>931</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D41" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E41" s="5">
+        <v>0.95825153935185181</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>14.2</v>
       </c>
@@ -2754,14 +3049,17 @@
       <c r="C42" s="3">
         <v>931</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D42" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E42" s="5">
+        <v>0.96930921296296291</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>14.1</v>
       </c>
@@ -2771,14 +3069,17 @@
       <c r="C43" s="3">
         <v>931</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D43" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E43" s="5">
+        <v>0.98036711805555565</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>14.1</v>
       </c>
@@ -2788,14 +3089,17 @@
       <c r="C44" s="3">
         <v>931</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D44" s="4">
+        <v>42530</v>
+      </c>
+      <c r="E44" s="5">
+        <v>0.99142873842592583</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>13.9</v>
       </c>
@@ -2805,14 +3109,17 @@
       <c r="C45" s="3">
         <v>931</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D45" s="4">
+        <v>42531</v>
+      </c>
+      <c r="E45" s="5">
+        <v>2.4826388888888888E-3</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>13.8</v>
       </c>
@@ -2822,14 +3129,17 @@
       <c r="C46" s="3">
         <v>931</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D46" s="4">
+        <v>42531</v>
+      </c>
+      <c r="E46" s="5">
+        <v>1.3540358796296297E-2</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>13.8</v>
       </c>
@@ -2839,14 +3149,17 @@
       <c r="C47" s="3">
         <v>931</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D47" s="4">
+        <v>42531</v>
+      </c>
+      <c r="E47" s="5">
+        <v>2.4598136574074076E-2</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>13.7</v>
       </c>
@@ -2856,14 +3169,17 @@
       <c r="C48" s="3">
         <v>931</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D48" s="4">
+        <v>42531</v>
+      </c>
+      <c r="E48" s="5">
+        <v>3.5655856481481486E-2</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>13.5</v>
       </c>
@@ -2873,14 +3189,17 @@
       <c r="C49" s="3">
         <v>931</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D49" s="4">
+        <v>42531</v>
+      </c>
+      <c r="E49" s="5">
+        <v>4.6713738425925931E-2</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>13.4</v>
       </c>
@@ -2890,11 +3209,314 @@
       <c r="C50" s="3">
         <v>931</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>100</v>
+      <c r="D50" s="4">
+        <v>42531</v>
+      </c>
+      <c r="E50" s="5">
+        <v>5.7771354166666671E-2</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>13.3</v>
+      </c>
+      <c r="B51" s="3">
+        <v>52.8</v>
+      </c>
+      <c r="C51" s="3">
+        <v>930</v>
+      </c>
+      <c r="D51" s="4">
+        <v>42531</v>
+      </c>
+      <c r="E51" s="5">
+        <v>6.882907407407407E-2</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>13.2</v>
+      </c>
+      <c r="B52" s="3">
+        <v>53.1</v>
+      </c>
+      <c r="C52" s="3">
+        <v>931</v>
+      </c>
+      <c r="D52" s="4">
+        <v>42531</v>
+      </c>
+      <c r="E52" s="5">
+        <v>7.9886817129629625E-2</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
+        <v>13.1</v>
+      </c>
+      <c r="B53" s="3">
+        <v>53.3</v>
+      </c>
+      <c r="C53" s="3">
+        <v>931</v>
+      </c>
+      <c r="D53" s="4">
+        <v>42531</v>
+      </c>
+      <c r="E53" s="5">
+        <v>9.0944594907407403E-2</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
+        <v>13.1</v>
+      </c>
+      <c r="B54" s="3">
+        <v>53.7</v>
+      </c>
+      <c r="C54" s="3">
+        <v>931</v>
+      </c>
+      <c r="D54" s="4">
+        <v>42531</v>
+      </c>
+      <c r="E54" s="5">
+        <v>0.10200362268518519</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <v>13</v>
+      </c>
+      <c r="B55" s="3">
+        <v>53.7</v>
+      </c>
+      <c r="C55" s="3">
+        <v>931</v>
+      </c>
+      <c r="D55" s="4">
+        <v>42531</v>
+      </c>
+      <c r="E55" s="5">
+        <v>0.11305983796296297</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <v>12.9</v>
+      </c>
+      <c r="B56" s="3">
+        <v>53.8</v>
+      </c>
+      <c r="C56" s="3">
+        <v>931</v>
+      </c>
+      <c r="D56" s="4">
+        <v>42531</v>
+      </c>
+      <c r="E56" s="5">
+        <v>0.12412620370370371</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
+        <v>12.8</v>
+      </c>
+      <c r="B57" s="3">
+        <v>54</v>
+      </c>
+      <c r="C57" s="3">
+        <v>931</v>
+      </c>
+      <c r="D57" s="4">
+        <v>42531</v>
+      </c>
+      <c r="E57" s="5">
+        <v>0.13517533564814815</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <v>12.8</v>
+      </c>
+      <c r="B58" s="3">
+        <v>54.3</v>
+      </c>
+      <c r="C58" s="3">
+        <v>931</v>
+      </c>
+      <c r="D58" s="4">
+        <v>42531</v>
+      </c>
+      <c r="E58" s="5">
+        <v>0.14623340277777777</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="3">
+        <v>12.7</v>
+      </c>
+      <c r="B59" s="3">
+        <v>54.7</v>
+      </c>
+      <c r="C59" s="3">
+        <v>931</v>
+      </c>
+      <c r="D59" s="4">
+        <v>42531</v>
+      </c>
+      <c r="E59" s="5">
+        <v>0.15729067129629629</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
+        <v>12.6</v>
+      </c>
+      <c r="B60" s="3">
+        <v>54.9</v>
+      </c>
+      <c r="C60" s="3">
+        <v>930</v>
+      </c>
+      <c r="D60" s="4">
+        <v>42531</v>
+      </c>
+      <c r="E60" s="5">
+        <v>0.16834828703703705</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="B61" s="3">
+        <v>55.4</v>
+      </c>
+      <c r="C61" s="3">
+        <v>930</v>
+      </c>
+      <c r="D61" s="4">
+        <v>42531</v>
+      </c>
+      <c r="E61" s="5">
+        <v>0.17940592592592594</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
+        <v>12.4</v>
+      </c>
+      <c r="B62" s="3">
+        <v>55.5</v>
+      </c>
+      <c r="C62" s="3">
+        <v>930</v>
+      </c>
+      <c r="D62" s="4">
+        <v>42531</v>
+      </c>
+      <c r="E62" s="5">
+        <v>0.19046371527777781</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
+        <v>12.3</v>
+      </c>
+      <c r="B63" s="3">
+        <v>55.6</v>
+      </c>
+      <c r="C63" s="3">
+        <v>930</v>
+      </c>
+      <c r="D63" s="4">
+        <v>42531</v>
+      </c>
+      <c r="E63" s="5">
+        <v>0.20152120370370372</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="3">
+        <v>12.1</v>
+      </c>
+      <c r="B64" s="3">
+        <v>56.1</v>
+      </c>
+      <c r="C64" s="3">
+        <v>930</v>
+      </c>
+      <c r="D64" s="4">
+        <v>42531</v>
+      </c>
+      <c r="E64" s="5">
+        <v>0.21257873842592592</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="3">
+        <v>11.9</v>
+      </c>
+      <c r="B65" s="3">
+        <v>56.7</v>
+      </c>
+      <c r="C65" s="3">
+        <v>930</v>
+      </c>
+      <c r="D65" s="4">
+        <v>42531</v>
+      </c>
+      <c r="E65" s="5">
+        <v>0.2236363888888889</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>